<commit_message>
add docstrings to SurveyCreator methods
</commit_message>
<xml_diff>
--- a/templates/survey-metadata-template.xlsx
+++ b/templates/survey-metadata-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahndi.minah/Desktop/gitcode/dev/frog_survey/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vahnd\Desktop\gitcode\quant-survey\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3263518-1AD7-2445-8FAA-1D1DCEA3B42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA88598-F06F-4AD8-BF90-6A9BC3AECDCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8400" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{C0BB3EEB-BB89-BE4A-AA61-584997E86E67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0BB3EEB-BB89-BE4A-AA61-584997E86E67}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="7" r:id="rId1"/>
@@ -144,8 +144,88 @@
     <t>categories</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">For categorical questions, enter the name of the category list here. The values for each category will be pulled from the </t>
+    <t>ordered</t>
+  </si>
+  <si>
+    <t>Only required for categorical questions. Enter TRUE if the category values are ordered and FALSE otherwise.</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>Contains a list of all the attributes in the survey, and references to their metadata, e.g. categories, in other sheets.</t>
+  </si>
+  <si>
+    <t>Name for the question. This will be the name of the property which accesses the question on the survey (or question group), so should be a valid Python variable.</t>
+  </si>
+  <si>
+    <t>The text of the attribute. This is typically the exact wording of the attribute question and is used for labelling axes in charts etc.</t>
+  </si>
+  <si>
+    <t>Optional regular expression to use to match the attribute column in the survey raw data file. Also can use for example if you want to abbreviate or otherwise change the attribute text.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter the type of attribute here e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MultiCategoryAttribute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Can also abbreviate e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MultiCategory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Only required for categorical attributes. Enter TRUE if the category values are ordered and FALSE otherwise.</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>Contains a list of every category, each with a list of its possible values. N.B. this is required even for unordered questions and attributes so that even if no respondent gives a particular response, it is still part of the question.</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Name for a list of categorical values. These names are referenced in the </t>
     </r>
     <r>
       <rPr>
@@ -156,17 +236,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column of the </t>
+      <t>categories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> columns of the </t>
     </r>
     <r>
       <rPr>
@@ -178,132 +258,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>orders</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sheet where the value in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>category</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column matches this name.</t>
-    </r>
-  </si>
-  <si>
-    <t>ordered</t>
-  </si>
-  <si>
-    <t>Only required for categorical questions. Enter TRUE if the category values are ordered and FALSE otherwise.</t>
-  </si>
-  <si>
-    <t>attributes</t>
-  </si>
-  <si>
-    <t>Contains a list of all the attributes in the survey, and references to their metadata, e.g. categories, in other sheets.</t>
-  </si>
-  <si>
-    <t>Name for the question. This will be the name of the property which accesses the question on the survey (or question group), so should be a valid Python variable.</t>
-  </si>
-  <si>
-    <t>The text of the attribute. This is typically the exact wording of the attribute question and is used for labelling axes in charts etc.</t>
-  </si>
-  <si>
-    <t>Optional regular expression to use to match the attribute column in the survey raw data file. Also can use for example if you want to abbreviate or otherwise change the attribute text.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enter the type of attribute here e.g. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MultiCategoryAttribute</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Can also abbreviate e.g. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MultiCategory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For categorical attributes, enter the name of the category list here. The values for each category will be pulled from the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column of the </t>
+      <t>questions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
     </r>
     <r>
       <rPr>
@@ -315,17 +280,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>orders</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sheet where the value in the </t>
+      <t>attributes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheets.</t>
+    </r>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Contains the values for each category set. The order listed will be the plot order of the corresponding categorical question(s) or attribute(s), whether or not the categorical question or attribute is ordered.</t>
+  </si>
+  <si>
+    <t>loop_expressions</t>
+  </si>
+  <si>
+    <t>Contains a list of regular expressions for each combination of loop variables in the questions sheet. There is an expression used to match all the questions in a loop, as well as an expression builder used to create  appropriately named questions and groups from loop values. (loop values are typically stored in the raw data file as numbers whereas loop variable values are names corresponding to the meaning of each loop instance).</t>
+  </si>
+  <si>
+    <t>loop_name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The name of the loop. This should be one or more loop_variables, separated by a new line. Each </t>
     </r>
     <r>
       <rPr>
@@ -336,34 +321,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>category</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column matches this name.</t>
-    </r>
-  </si>
-  <si>
-    <t>Only required for categorical attributes. Enter TRUE if the category values are ordered and FALSE otherwise.</t>
-  </si>
-  <si>
-    <t>orders</t>
-  </si>
-  <si>
-    <t>Contains a list of every category, each with a list of its possible values. N.B. this is required even for unordered questions and attributes so that even if no respondent gives a particular response, it is still part of the question.</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Name for a list of categorical values. These names are referenced in the </t>
+      <t>loop_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should correspond to one or more entries in the </t>
     </r>
     <r>
       <rPr>
@@ -374,17 +342,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>categories</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> columns of the </t>
+      <t>loop_variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column of the </t>
     </r>
     <r>
       <rPr>
@@ -406,7 +374,217 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and </t>
+      <t xml:space="preserve"> sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A regular expression which will be used to match questions which are part of the associated </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loop_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. There can be multiple expressions for each </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loop_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, as long as each question is matched only once. The number of parenthesis groups in the expression should be the same as the number of loop_variables in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loop_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and in the same order, since these will be extracted as the value of each loop_variable for matching questions.</t>
+    </r>
+  </si>
+  <si>
+    <t>expression_builder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A string which can be used to build a regular expression that will match the question associated with the values of the variables in a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loop_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Generally this should be the same as the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, but with each </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(group)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> replaced by the associated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{{variable_name}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>loop_mappings</t>
+  </si>
+  <si>
+    <t>Used to map from loop values (typically numbers) in the raw data file to value names so that the question and group names are more meaningful.</t>
+  </si>
+  <si>
+    <t>loop_variable</t>
+  </si>
+  <si>
+    <t>The name of the loop variable to map.</t>
+  </si>
+  <si>
+    <t>map_from</t>
+  </si>
+  <si>
+    <t>The value to map from, typically a number.</t>
+  </si>
+  <si>
+    <t>map_to</t>
+  </si>
+  <si>
+    <t>The value to map to, typically a variable value.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For categorical questions, enter the name of the category list here. The values for each category will be pulled from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column of the </t>
     </r>
     <r>
       <rPr>
@@ -418,37 +596,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>attributes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sheets.</t>
-    </r>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Contains the values for each category set. The order listed will be the plot order of the corresponding categorical question(s) or attribute(s), whether or not the categorical question or attribute is ordered.</t>
-  </si>
-  <si>
-    <t>loop_expressions</t>
-  </si>
-  <si>
-    <t>Contains a list of regular expressions for each combination of loop variables in the questions sheet. There is an expression used to match all the questions in a loop, as well as an expression builder used to create  appropriately named questions and groups from loop values. (loop values are typically stored in the raw data file as numbers whereas loop variable values are names corresponding to the meaning of each loop instance).</t>
-  </si>
-  <si>
-    <t>loop_name</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The name of the loop. This should be one or more loop_variables, separated by a new line. Each </t>
+      <t>orders</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet where the value in the </t>
     </r>
     <r>
       <rPr>
@@ -459,17 +617,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>loop_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> should correspond to one or more entries in the </t>
+      <t>category</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column matches this name.
+Category names must not overlap with the name of any question or attribute.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For categorical attributes, enter the name of the category list here. The values for each category will be pulled from the </t>
     </r>
     <r>
       <rPr>
@@ -480,7 +644,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>loop_variables</t>
+      <t>value</t>
     </r>
     <r>
       <rPr>
@@ -502,22 +666,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>questions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sheet.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A regular expression which will be used to match questions which are part of the associated </t>
+      <t>orders</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet where the value in the </t>
     </r>
     <r>
       <rPr>
@@ -528,176 +687,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>loop_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. There can be multiple expressions for each </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>loop_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, as long as each question is matched only once. The number of parenthesis groups in the expression should be the same as the number of loop_variables in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>loop_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and in the same order, since these will be extracted as the value of each loop_variable for matching questions.</t>
-    </r>
-  </si>
-  <si>
-    <t>expression_builder</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A string which can be used to build a regular expression that will match the question associated with the values of the variables in a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>loop_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Generally this should be the same as the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>expression</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, but with each </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(group)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> replaced by the associated </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{{variable_name}}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>loop_mappings</t>
-  </si>
-  <si>
-    <t>Used to map from loop values (typically numbers) in the raw data file to value names so that the question and group names are more meaningful.</t>
-  </si>
-  <si>
-    <t>loop_variable</t>
-  </si>
-  <si>
-    <t>The name of the loop variable to map.</t>
-  </si>
-  <si>
-    <t>map_from</t>
-  </si>
-  <si>
-    <t>The value to map from, typically a number.</t>
-  </si>
-  <si>
-    <t>map_to</t>
-  </si>
-  <si>
-    <t>The value to map to, typically a variable value.</t>
+      <t>category</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column matches this name.
+Category names must not overlap with the name of any question or attribute.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -941,6 +943,21 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -955,21 +972,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1297,21 +1299,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C416CB8-702A-314E-9161-CCC4F49BE6AC}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="217" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="19.625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="10" hidden="1"/>
+    <col min="5" max="16384" width="10.875" style="10" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1325,11 +1327,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:4" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="30" t="s">
@@ -1339,9 +1341,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
+    <row r="3" spans="1:4" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="30" t="s">
         <v>8</v>
       </c>
@@ -1349,9 +1351,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
+    <row r="4" spans="1:4" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
@@ -1359,9 +1361,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="30" t="s">
         <v>12</v>
       </c>
@@ -1369,9 +1371,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="30" t="s">
         <v>14</v>
       </c>
@@ -1379,195 +1381,195 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="30" t="s">
+      <c r="D8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="25" t="s">
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="41"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="31" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="41"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="31" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="41"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="41"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="31" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="26" t="s">
+      <c r="B15" s="37" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+      <c r="C15" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="D15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="32" t="s">
+    </row>
+    <row r="16" spans="1:4" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D16" s="27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="32" t="s">
+    <row r="17" spans="1:4" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="B17" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
+      <c r="C17" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="D17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="43"/>
+    </row>
+    <row r="18" spans="1:4" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A18" s="44"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="33" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="44"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="33" t="s">
+    <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="B20" s="39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="40" t="s">
+      <c r="C20" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="D20" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="34" t="s">
+    </row>
+    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D21" s="29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="34" t="s">
+    <row r="22" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D22" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1578,26 +1580,26 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="45.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="45.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="45.33203125" style="13"/>
+    <col min="8" max="16384" width="45.375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1617,7 +1619,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1639,17 +1641,17 @@
       <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1666,58 +1668,58 @@
         <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="10"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="10"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="10"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="10"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="10"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="10"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
@@ -1739,1007 +1741,1007 @@
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="15"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="16"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="16"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="16"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="16"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="16"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="7"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="7"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="7"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="7"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="7"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="7"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="7"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="7"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="7"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="7"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="7"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="7"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="7"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="7"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="7"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="7"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="7"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="7"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="7"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="7"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="7"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="7"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="7"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="7"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="7"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="7"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="7"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="7"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="7"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="7"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="7"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="7"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="7"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="7"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="7"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="7"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="7"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="7"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="7"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="7"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="7"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="7"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="7"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="7"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="7"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="7"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="7"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="7"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="7"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="7"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="7"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="7"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="7"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="7"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="7"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="7"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="7"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="7"/>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="7"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="7"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="7"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="10"/>
       <c r="B116" s="7"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="7"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="10"/>
       <c r="B119" s="7"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="7"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="7"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="7"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="10"/>
       <c r="B123" s="7"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="10"/>
       <c r="B124" s="7"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="10"/>
       <c r="B125" s="7"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
       <c r="B126" s="7"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="10"/>
       <c r="B127" s="7"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="10"/>
       <c r="B128" s="7"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
       <c r="B129" s="7"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
       <c r="B130" s="7"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="10"/>
       <c r="B131" s="7"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="10"/>
       <c r="B132" s="7"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="7"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="7"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="10"/>
       <c r="B135" s="7"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="10"/>
       <c r="B136" s="7"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="10"/>
       <c r="B137" s="7"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="10"/>
       <c r="B138" s="7"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="10"/>
       <c r="B139" s="7"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="10"/>
       <c r="B140" s="7"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="10"/>
       <c r="B141" s="7"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="10"/>
       <c r="B142" s="7"/>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="7"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="7"/>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="10"/>
       <c r="B145" s="7"/>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="10"/>
       <c r="B146" s="7"/>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="10"/>
       <c r="B147" s="7"/>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="10"/>
       <c r="B148" s="7"/>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="10"/>
       <c r="B149" s="7"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="10"/>
       <c r="B150" s="7"/>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="10"/>
       <c r="B151" s="10"/>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="10"/>
       <c r="B152" s="7"/>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="10"/>
       <c r="B153" s="7"/>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="10"/>
       <c r="B154" s="7"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="10"/>
       <c r="B155" s="7"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="10"/>
       <c r="B156" s="7"/>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="10"/>
       <c r="B157" s="7"/>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="10"/>
       <c r="B158" s="7"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="10"/>
       <c r="B159" s="7"/>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="10"/>
       <c r="B160" s="7"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="10"/>
       <c r="B161" s="7"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="10"/>
       <c r="B162" s="7"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="10"/>
       <c r="B163" s="7"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="10"/>
       <c r="B164" s="7"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="10"/>
       <c r="B165" s="7"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="10"/>
       <c r="B166" s="7"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="7"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="10"/>
       <c r="B168" s="7"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="10"/>
       <c r="B169" s="7"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="10"/>
       <c r="B170" s="7"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="10"/>
       <c r="B171" s="7"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="10"/>
       <c r="B172" s="7"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
       <c r="B173" s="7"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
       <c r="B174" s="7"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
       <c r="B175" s="7"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="10"/>
       <c r="B176" s="7"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
       <c r="B177" s="7"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
       <c r="B178" s="7"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="10"/>
       <c r="B179" s="7"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="10"/>
       <c r="B180" s="7"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="10"/>
       <c r="B181" s="7"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="10"/>
       <c r="B182" s="7"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="10"/>
       <c r="B183" s="7"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="10"/>
       <c r="B184" s="7"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="10"/>
       <c r="B185" s="7"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="10"/>
       <c r="B186" s="7"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="10"/>
       <c r="B187" s="7"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="10"/>
       <c r="B188" s="7"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="10"/>
       <c r="B189" s="7"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="10"/>
       <c r="B190" s="7"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="10"/>
       <c r="B191" s="7"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="10"/>
       <c r="B192" s="7"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="10"/>
       <c r="B193" s="7"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="10"/>
       <c r="B194" s="7"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="10"/>
       <c r="B195" s="7"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="10"/>
       <c r="B196" s="7"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="10"/>
       <c r="B197" s="7"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="10"/>
       <c r="B198" s="7"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="10"/>
       <c r="B199" s="7"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="10"/>
       <c r="B200" s="7"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="10"/>
       <c r="B201" s="7"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B202"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B204"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B205"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B207"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B210"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B220"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B221"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B222"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B223"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B224"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B228"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B229"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B231"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B232"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B234"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B235"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B237"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B238"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B258"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B259"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B261"/>
     </row>
   </sheetData>
@@ -2761,33 +2763,33 @@
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="C4" s="10"/>
     </row>
@@ -2809,26 +2811,26 @@
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="15.83203125" style="10"/>
+    <col min="4" max="16384" width="15.875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="9" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{D4B68E45-EF3F-0A42-9068-063F7FE5AC8C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3053,18 +3055,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3087,14 +3089,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B064398-A2C5-4EDD-938E-E1124410CBBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E143621C-B52A-45E4-96E2-199122A6FBD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3109,4 +3103,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B064398-A2C5-4EDD-938E-E1124410CBBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>